<commit_message>
determinstic and bio monte loop both seem to be stable, after redoing dimensions
</commit_message>
<xml_diff>
--- a/sheets/input/tests/FR_Input_st_small_Var.xlsx
+++ b/sheets/input/tests/FR_Input_st_small_Var.xlsx
@@ -56,334 +56,334 @@
     <t>U, Normal</t>
   </si>
   <si>
-    <t>13.0, 0.65</t>
+    <t>13.0, 0.13</t>
   </si>
   <si>
     <t>Concentration of Dissolved Organic Carbon Content (kg/L)</t>
   </si>
   <si>
-    <t>2.2e-06, 1.1e-07</t>
+    <t>2.2e-06, 2.2e-08</t>
   </si>
   <si>
     <t>Concentration of Particulate Organic Carbon Content (kg/L)</t>
   </si>
   <si>
-    <t>5.4e-07, 2.7e-08</t>
+    <t>5.4e-07, 5.4e-09</t>
   </si>
   <si>
     <t>Concentration of suspended solids in water (g/L)</t>
   </si>
   <si>
+    <t>4e-05, 4e-07</t>
+  </si>
+  <si>
+    <t>Fraction of Organic Carbon Content in Sediment</t>
+  </si>
+  <si>
+    <t>0.071, 0.00071</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen saturation</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen concentration (if avaliable) (mg O2/L)</t>
+  </si>
+  <si>
+    <t>POC–octanol proportionality constant (deafult = .08)</t>
+  </si>
+  <si>
+    <t>DOC–octanol proportionality constant (deafult = .35)</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>Chemical</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Bad Chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Octanol-Water Partition Coefficent </t>
+  </si>
+  <si>
+    <t>5.75, 0.2875</t>
+  </si>
+  <si>
+    <t>Concentration in Sediment (ng/g)</t>
+  </si>
+  <si>
+    <t>2.307, 0.11535</t>
+  </si>
+  <si>
+    <t>Total Concentration in Water (g/L) (if avaliable)</t>
+  </si>
+  <si>
+    <t>0.013, 0.00065</t>
+  </si>
+  <si>
+    <t>Dissolved Concentration in Water (g/L) (if avaliable)</t>
+  </si>
+  <si>
+    <t>Disequilbrium factor of Disolved Organic Carbon (if avaliable)</t>
+  </si>
+  <si>
+    <t>Disequilbrium factor of Particulate Organic Carbon (if avaliable)</t>
+  </si>
+  <si>
+    <t>Extra Bad Chemical</t>
+  </si>
+  <si>
+    <t>6.0, 0.3</t>
+  </si>
+  <si>
+    <t>1.997, 0.09985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Concentration in Water (g/L) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Fish/Inverterbrate</t>
+  </si>
+  <si>
+    <t>Zooplankton</t>
+  </si>
+  <si>
+    <t>Phytoplankton</t>
+  </si>
+  <si>
+    <t>Zebra Mussel</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>0.00011, 5.5e-06</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>V, Normal</t>
+  </si>
+  <si>
+    <t>5.7e-08, 2.85e-09</t>
+  </si>
+  <si>
+    <t>Growth Rate (d^-1)</t>
+  </si>
+  <si>
+    <t>0.08, 0.004</t>
+  </si>
+  <si>
+    <t>Lipid Content (kg/kg)</t>
+  </si>
+  <si>
+    <t>0.012, 0.0006</t>
+  </si>
+  <si>
+    <t>Lipid Content (deafult = .005) (kg/kg)</t>
+  </si>
+  <si>
+    <t>Non-Lipid Content (deafult = .2) (kg/kg)</t>
+  </si>
+  <si>
+    <t>Non-Lipid Content (deafult = .065) (kg/kg)</t>
+  </si>
+  <si>
+    <t>Fraction Pore Water Ventilated</t>
+  </si>
+  <si>
+    <t>0.05, 0.0025</t>
+  </si>
+  <si>
+    <t>Fraction Pore Water Ventilated (deafult = 0)</t>
+  </si>
+  <si>
+    <t>Feeding Rate (if avaliable) (kg/d)</t>
+  </si>
+  <si>
+    <t>Dietary absorption efficency of lipid Organic Matter (deafult  = .72)</t>
+  </si>
+  <si>
+    <t>Dietary absorption efficency of lipid Organic Matter (deafult  = .75)</t>
+  </si>
+  <si>
+    <t>Dietary absorption efficency of nonlipid Organic Matter (deafult  = .72)</t>
+  </si>
+  <si>
+    <t>Dietary absorption efficency of nonlipid Organic Matter (deafult  = .75)</t>
+  </si>
+  <si>
+    <t>Dietary absorption efficency of water (deafult  = .25)</t>
+  </si>
+  <si>
+    <t>Dietary absorption efficency of water (deafult  = .50)</t>
+  </si>
+  <si>
+    <t>Feeding Rate (if avaliable)(kg/d)</t>
+  </si>
+  <si>
+    <t>Growth Rate (if known) (d^-1)</t>
+  </si>
+  <si>
+    <t>Filter Feeder Flag (0 = is, and 1 = is not)</t>
+  </si>
+  <si>
+    <t>Caddisfly larvae</t>
+  </si>
+  <si>
     <t>4e-05, 2e-06</t>
   </si>
   <si>
-    <t>Fraction of Organic Carbon Content in Sediment</t>
+    <t>0.017, 0.00085</t>
+  </si>
+  <si>
+    <t>Growth Rate Iif known) (d^-1)</t>
+  </si>
+  <si>
+    <t>Mayfly</t>
+  </si>
+  <si>
+    <t>0.0001, 5e-06</t>
+  </si>
+  <si>
+    <t>0.02, 0.001</t>
+  </si>
+  <si>
+    <t>Gammarus</t>
+  </si>
+  <si>
+    <t>1e-05, 5e-07</t>
+  </si>
+  <si>
+    <t>0.021, 0.00105</t>
+  </si>
+  <si>
+    <t>Crayfish</t>
+  </si>
+  <si>
+    <t>0.0018, 9e-05</t>
+  </si>
+  <si>
+    <t>0.019, 0.00095</t>
+  </si>
+  <si>
+    <t>YoY</t>
+  </si>
+  <si>
+    <t>0.0004, 2e-05</t>
+  </si>
+  <si>
+    <t>Emerald shiner</t>
+  </si>
+  <si>
+    <t>0.0025, 0.000125</t>
+  </si>
+  <si>
+    <t>0.047, 0.00235</t>
+  </si>
+  <si>
+    <t>Alewife</t>
+  </si>
+  <si>
+    <t>0.116, 0.0058</t>
+  </si>
+  <si>
+    <t>0.074, 0.0037</t>
+  </si>
+  <si>
+    <t>Trout-perch</t>
+  </si>
+  <si>
+    <t>0.0068, 0.00034</t>
+  </si>
+  <si>
+    <t>0.029, 0.00145</t>
+  </si>
+  <si>
+    <t>Small White Sucker</t>
+  </si>
+  <si>
+    <t>0.055, 0.00275</t>
+  </si>
+  <si>
+    <t>Black Crappie</t>
+  </si>
+  <si>
+    <t>0.0696, 0.00348</t>
+  </si>
+  <si>
+    <t>0.057, 0.00285</t>
+  </si>
+  <si>
+    <t>White Perch</t>
+  </si>
+  <si>
+    <t>0.056, 0.0028</t>
+  </si>
+  <si>
+    <t>Yellow Perch</t>
+  </si>
+  <si>
+    <t>0.036, 0.0018</t>
+  </si>
+  <si>
+    <t>Adult white sucker</t>
+  </si>
+  <si>
+    <t>0.87, 0.0435</t>
+  </si>
+  <si>
+    <t>0.081, 0.00405</t>
+  </si>
+  <si>
+    <t>Freshwater drum</t>
+  </si>
+  <si>
+    <t>0.547, 0.02735</t>
   </si>
   <si>
     <t>0.071, 0.00355</t>
   </si>
   <si>
-    <t>Dissolved oxygen saturation</t>
-  </si>
-  <si>
-    <t>Dissolved oxygen concentration (if avaliable) (mg O2/L)</t>
-  </si>
-  <si>
-    <t>POC–octanol proportionality constant (deafult = .08)</t>
-  </si>
-  <si>
-    <t>DOC–octanol proportionality constant (deafult = .35)</t>
-  </si>
-  <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>Chemical</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Bad Chemical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Octanol-Water Partition Coefficent </t>
-  </si>
-  <si>
-    <t>5.75, 2.875</t>
-  </si>
-  <si>
-    <t>Concentration in Sediment (ng/g)</t>
-  </si>
-  <si>
-    <t>2.307, 1.1535</t>
-  </si>
-  <si>
-    <t>Total Concentration in Water (g/L) (if avaliable)</t>
-  </si>
-  <si>
-    <t>0.013, 0.0065</t>
-  </si>
-  <si>
-    <t>Dissolved Concentration in Water (g/L) (if avaliable)</t>
-  </si>
-  <si>
-    <t>Disequilbrium factor of Disolved Organic Carbon (if avaliable)</t>
-  </si>
-  <si>
-    <t>Disequilbrium factor of Particulate Organic Carbon (if avaliable)</t>
-  </si>
-  <si>
-    <t>Extra Bad Chemical</t>
-  </si>
-  <si>
-    <t>6.0, 3.0</t>
-  </si>
-  <si>
-    <t>1.997, 0.9985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Concentration in Water (g/L) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Fish/Inverterbrate</t>
-  </si>
-  <si>
-    <t>Zooplankton</t>
-  </si>
-  <si>
-    <t>Phytoplankton</t>
-  </si>
-  <si>
-    <t>Zebra Mussel</t>
-  </si>
-  <si>
-    <t>Weight (kg)</t>
-  </si>
-  <si>
-    <t>0.00011, 5.5e-05</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>V, Normal</t>
-  </si>
-  <si>
-    <t>5.7e-08, 2.85e-08</t>
-  </si>
-  <si>
-    <t>Growth Rate (d^-1)</t>
-  </si>
-  <si>
-    <t>0.08, 0.04</t>
-  </si>
-  <si>
-    <t>Lipid Content (kg/kg)</t>
-  </si>
-  <si>
-    <t>0.012, 0.006</t>
-  </si>
-  <si>
-    <t>Lipid Content (deafult = .005) (kg/kg)</t>
-  </si>
-  <si>
-    <t>Non-Lipid Content (deafult = .2) (kg/kg)</t>
-  </si>
-  <si>
-    <t>Non-Lipid Content (deafult = .065) (kg/kg)</t>
-  </si>
-  <si>
-    <t>Fraction Pore Water Ventilated</t>
-  </si>
-  <si>
-    <t>0.05, 0.025</t>
-  </si>
-  <si>
-    <t>Fraction Pore Water Ventilated (deafult = 0)</t>
-  </si>
-  <si>
-    <t>Feeding Rate (if avaliable) (kg/d)</t>
-  </si>
-  <si>
-    <t>Dietary absorption efficency of lipid Organic Matter (deafult  = .72)</t>
-  </si>
-  <si>
-    <t>Dietary absorption efficency of lipid Organic Matter (deafult  = .75)</t>
-  </si>
-  <si>
-    <t>Dietary absorption efficency of nonlipid Organic Matter (deafult  = .72)</t>
-  </si>
-  <si>
-    <t>Dietary absorption efficency of nonlipid Organic Matter (deafult  = .75)</t>
-  </si>
-  <si>
-    <t>Dietary absorption efficency of water (deafult  = .25)</t>
-  </si>
-  <si>
-    <t>Dietary absorption efficency of water (deafult  = .50)</t>
-  </si>
-  <si>
-    <t>Feeding Rate (if avaliable)(kg/d)</t>
-  </si>
-  <si>
-    <t>Growth Rate (if known) (d^-1)</t>
-  </si>
-  <si>
-    <t>Filter Feeder Flag (0 = is, and 1 = is not)</t>
-  </si>
-  <si>
-    <t>Caddisfly larvae</t>
-  </si>
-  <si>
-    <t>4e-05, 2e-05</t>
-  </si>
-  <si>
-    <t>0.017, 0.0085</t>
-  </si>
-  <si>
-    <t>Growth Rate Iif known) (d^-1)</t>
-  </si>
-  <si>
-    <t>Mayfly</t>
-  </si>
-  <si>
-    <t>0.0001, 5e-05</t>
-  </si>
-  <si>
-    <t>0.02, 0.01</t>
-  </si>
-  <si>
-    <t>Gammarus</t>
-  </si>
-  <si>
-    <t>1e-05, 5e-06</t>
-  </si>
-  <si>
-    <t>0.021, 0.0105</t>
-  </si>
-  <si>
-    <t>Crayfish</t>
-  </si>
-  <si>
-    <t>0.0018, 0.0009</t>
-  </si>
-  <si>
-    <t>0.019, 0.0095</t>
-  </si>
-  <si>
-    <t>YoY</t>
-  </si>
-  <si>
-    <t>0.0004, 0.0002</t>
-  </si>
-  <si>
-    <t>Emerald shiner</t>
-  </si>
-  <si>
-    <t>0.0025, 0.00125</t>
-  </si>
-  <si>
-    <t>0.047, 0.0235</t>
-  </si>
-  <si>
-    <t>Alewife</t>
-  </si>
-  <si>
-    <t>0.116, 0.058</t>
-  </si>
-  <si>
-    <t>0.074, 0.037</t>
-  </si>
-  <si>
-    <t>Trout-perch</t>
-  </si>
-  <si>
-    <t>0.0068, 0.0034</t>
-  </si>
-  <si>
-    <t>0.029, 0.0145</t>
-  </si>
-  <si>
-    <t>Small White Sucker</t>
-  </si>
-  <si>
-    <t>0.055, 0.0275</t>
-  </si>
-  <si>
-    <t>Black Crappie</t>
-  </si>
-  <si>
-    <t>0.0696, 0.0348</t>
-  </si>
-  <si>
-    <t>0.057, 0.0285</t>
-  </si>
-  <si>
-    <t>White Perch</t>
-  </si>
-  <si>
-    <t>0.056, 0.028</t>
-  </si>
-  <si>
-    <t>Yellow Perch</t>
-  </si>
-  <si>
-    <t>0.036, 0.018</t>
-  </si>
-  <si>
-    <t>Adult white sucker</t>
-  </si>
-  <si>
-    <t>0.87, 0.435</t>
-  </si>
-  <si>
-    <t>0.081, 0.0405</t>
-  </si>
-  <si>
-    <t>Freshwater drum</t>
-  </si>
-  <si>
-    <t>0.547, 0.2735</t>
-  </si>
-  <si>
-    <t>0.071, 0.0355</t>
-  </si>
-  <si>
     <t>Gizzard shad</t>
   </si>
   <si>
-    <t>0.585, 0.2925</t>
-  </si>
-  <si>
-    <t>0.075, 0.0375</t>
+    <t>0.585, 0.02925</t>
+  </si>
+  <si>
+    <t>0.075, 0.00375</t>
   </si>
   <si>
     <t>Small mouth bass</t>
   </si>
   <si>
-    <t>0.715, 0.3575</t>
+    <t>0.715, 0.03575</t>
   </si>
   <si>
     <t>Large mouth bass</t>
   </si>
   <si>
-    <t>0.536, 0.268</t>
+    <t>0.536, 0.0268</t>
   </si>
   <si>
     <t>Walleye</t>
   </si>
   <si>
-    <t>1.33, 0.665</t>
-  </si>
-  <si>
-    <t>0.1, 0.05</t>
+    <t>1.33, 0.0665</t>
+  </si>
+  <si>
+    <t>0.1, 0.005</t>
   </si>
   <si>
     <t>Diet</t>
@@ -404,118 +404,118 @@
     <t>Percentage of diet</t>
   </si>
   <si>
-    <t>5.75, 0.2875</t>
-  </si>
-  <si>
-    <t>2.307, 0.11535</t>
-  </si>
-  <si>
-    <t>0.013, 0.00065</t>
-  </si>
-  <si>
-    <t>6.0, 0.3</t>
-  </si>
-  <si>
-    <t>1.997, 0.09985</t>
-  </si>
-  <si>
-    <t>0.00011, 5.5e-06</t>
-  </si>
-  <si>
-    <t>0.05, 0.0025</t>
-  </si>
-  <si>
-    <t>0.017, 0.00085</t>
-  </si>
-  <si>
-    <t>0.0001, 5e-06</t>
-  </si>
-  <si>
-    <t>0.02, 0.001</t>
-  </si>
-  <si>
-    <t>1e-05, 5e-07</t>
-  </si>
-  <si>
-    <t>0.021, 0.00105</t>
-  </si>
-  <si>
-    <t>0.0018, 9e-05</t>
-  </si>
-  <si>
-    <t>0.019, 0.00095</t>
-  </si>
-  <si>
-    <t>0.0004, 2e-05</t>
-  </si>
-  <si>
-    <t>0.0025, 0.000125</t>
-  </si>
-  <si>
-    <t>0.047, 0.00235</t>
-  </si>
-  <si>
-    <t>0.116, 0.0058</t>
-  </si>
-  <si>
-    <t>0.074, 0.0037</t>
-  </si>
-  <si>
-    <t>0.0068, 0.00034</t>
-  </si>
-  <si>
-    <t>0.029, 0.00145</t>
-  </si>
-  <si>
-    <t>0.055, 0.00275</t>
-  </si>
-  <si>
-    <t>0.0696, 0.00348</t>
-  </si>
-  <si>
-    <t>0.057, 0.00285</t>
-  </si>
-  <si>
-    <t>0.056, 0.0028</t>
-  </si>
-  <si>
-    <t>0.036, 0.0018</t>
-  </si>
-  <si>
-    <t>0.87, 0.0435</t>
-  </si>
-  <si>
-    <t>0.081, 0.00405</t>
-  </si>
-  <si>
-    <t>0.547, 0.02735</t>
-  </si>
-  <si>
-    <t>0.585, 0.02925</t>
-  </si>
-  <si>
-    <t>0.075, 0.00375</t>
-  </si>
-  <si>
-    <t>0.715, 0.03575</t>
-  </si>
-  <si>
-    <t>0.536, 0.0268</t>
-  </si>
-  <si>
-    <t>1.33, 0.0665</t>
-  </si>
-  <si>
-    <t>0.1, 0.005</t>
-  </si>
-  <si>
-    <t>5.7e-08, 2.85e-09</t>
-  </si>
-  <si>
-    <t>0.012, 0.0006</t>
-  </si>
-  <si>
-    <t>0.08, 0.004</t>
+    <t>5.75, 0.0575</t>
+  </si>
+  <si>
+    <t>2.307, 0.02307</t>
+  </si>
+  <si>
+    <t>0.013, 0.00013</t>
+  </si>
+  <si>
+    <t>6.0, 0.06</t>
+  </si>
+  <si>
+    <t>1.997, 0.01997</t>
+  </si>
+  <si>
+    <t>0.00011, 1.1e-06</t>
+  </si>
+  <si>
+    <t>0.05, 0.0005</t>
+  </si>
+  <si>
+    <t>0.017, 0.00017</t>
+  </si>
+  <si>
+    <t>0.0001, 1e-06</t>
+  </si>
+  <si>
+    <t>0.02, 0.0002</t>
+  </si>
+  <si>
+    <t>1e-05, 1e-07</t>
+  </si>
+  <si>
+    <t>0.021, 0.00021</t>
+  </si>
+  <si>
+    <t>0.0018, 1.8e-05</t>
+  </si>
+  <si>
+    <t>0.019, 0.00019</t>
+  </si>
+  <si>
+    <t>0.0004, 4e-06</t>
+  </si>
+  <si>
+    <t>0.0025, 2.5e-05</t>
+  </si>
+  <si>
+    <t>0.047, 0.00047</t>
+  </si>
+  <si>
+    <t>0.116, 0.00116</t>
+  </si>
+  <si>
+    <t>0.074, 0.00074</t>
+  </si>
+  <si>
+    <t>0.0068, 6.8e-05</t>
+  </si>
+  <si>
+    <t>0.029, 0.00029</t>
+  </si>
+  <si>
+    <t>0.055, 0.00055</t>
+  </si>
+  <si>
+    <t>0.0696, 0.000696</t>
+  </si>
+  <si>
+    <t>0.057, 0.00057</t>
+  </si>
+  <si>
+    <t>0.056, 0.00056</t>
+  </si>
+  <si>
+    <t>0.036, 0.00036</t>
+  </si>
+  <si>
+    <t>0.87, 0.0087</t>
+  </si>
+  <si>
+    <t>0.081, 0.00081</t>
+  </si>
+  <si>
+    <t>0.547, 0.00547</t>
+  </si>
+  <si>
+    <t>0.585, 0.00585</t>
+  </si>
+  <si>
+    <t>0.075, 0.00075</t>
+  </si>
+  <si>
+    <t>0.715, 0.00715</t>
+  </si>
+  <si>
+    <t>0.536, 0.00536</t>
+  </si>
+  <si>
+    <t>1.33, 0.0133</t>
+  </si>
+  <si>
+    <t>0.1, 0.001</t>
+  </si>
+  <si>
+    <t>5.7e-08, 5.7e-10</t>
+  </si>
+  <si>
+    <t>0.012, 0.00012</t>
+  </si>
+  <si>
+    <t>0.08, 0.0008</t>
   </si>
 </sst>
 </file>

</xml_diff>